<commit_message>
Eni materials planning mode
</commit_message>
<xml_diff>
--- a/examples/Utopia2_planning_single_node_DN/sets/global.xlsx
+++ b/examples/Utopia2_planning_single_node_DN/sets/global.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466488AD-8DC2-9441-878C-563C271BA450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>Year</t>
   </si>
@@ -28,9 +27,21 @@
     <t>Year_name</t>
   </si>
   <si>
+    <t>Y0</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
     <t>Region</t>
   </si>
   <si>
+    <t>reg1</t>
+  </si>
+  <si>
     <t>Carrier</t>
   </si>
   <si>
@@ -40,9 +51,21 @@
     <t>Carr_type</t>
   </si>
   <si>
+    <t>Elec</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
     <t>Region_name</t>
   </si>
   <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -52,6 +75,15 @@
     <t>Tech_category</t>
   </si>
   <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Electricity Transmission Line</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
     <t>Timeslice</t>
   </si>
   <si>
@@ -59,12 +91,144 @@
   </si>
   <si>
     <t>Timeslice_fraction</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>Diesel Pipeline</t>
+  </si>
+  <si>
+    <t>Utopia</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>Y7</t>
+  </si>
+  <si>
+    <t>Y8</t>
+  </si>
+  <si>
+    <t>Y9</t>
+  </si>
+  <si>
+    <t>Y10</t>
+  </si>
+  <si>
+    <t>Oil Resource Extraction</t>
+  </si>
+  <si>
+    <t>Oil Refinery</t>
+  </si>
+  <si>
+    <t>Oil_extr</t>
+  </si>
+  <si>
+    <t>Oil_refine</t>
+  </si>
+  <si>
+    <t>Oil_PP</t>
+  </si>
+  <si>
+    <t>Oil Power Plant</t>
+  </si>
+  <si>
+    <t>Hydro_PP</t>
+  </si>
+  <si>
+    <t>Hydro Power Plant</t>
+  </si>
+  <si>
+    <t>Elec_transmission</t>
+  </si>
+  <si>
+    <t>Diesel_pipeline</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>ICEV</t>
+  </si>
+  <si>
+    <t>HH_elec_demand</t>
+  </si>
+  <si>
+    <t>Other_elec_demand</t>
+  </si>
+  <si>
+    <t>Electric Vehicles Demand</t>
+  </si>
+  <si>
+    <t>ICE Vehicles Demand</t>
+  </si>
+  <si>
+    <t>Household Elecricity Demand</t>
+  </si>
+  <si>
+    <t>Other Electricity Demand</t>
+  </si>
+  <si>
+    <t>Raw Oil</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Oil_final</t>
+  </si>
+  <si>
+    <t>Elec_final</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Final Diesel Oil</t>
+  </si>
+  <si>
+    <t>Final Electricity</t>
+  </si>
+  <si>
+    <t>WD_days</t>
+  </si>
+  <si>
+    <t>WD_nights</t>
+  </si>
+  <si>
+    <t>WE_days</t>
+  </si>
+  <si>
+    <t>WE_nights</t>
+  </si>
+  <si>
+    <t>Weekdays-nights</t>
+  </si>
+  <si>
+    <t>Weekends-days</t>
+  </si>
+  <si>
+    <t>Weekdays-days</t>
+  </si>
+  <si>
+    <t>Weekends-nights</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,58 +668,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Years" displayName="Years" ref="A5:B16" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="A5:B16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Years" displayName="Years" ref="A5:B16" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A5:B16"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Year" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Year_name" dataDxfId="20"/>
+    <tableColumn id="2" name="Year" dataDxfId="21"/>
+    <tableColumn id="3" name="Year_name" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Regions" displayName="Regions" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Regions" displayName="Regions" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Region"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Region_name"/>
+    <tableColumn id="1" name="Region"/>
+    <tableColumn id="2" name="Region_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Technologies_glob" displayName="Technologies_glob" ref="A19:C29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A19:C29" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Technologies_glob" displayName="Technologies_glob" ref="A19:C29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A19:C29"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Technology" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Tech_name" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Tech_category" dataDxfId="12"/>
+    <tableColumn id="2" name="Technology" dataDxfId="14"/>
+    <tableColumn id="3" name="Tech_name" dataDxfId="13"/>
+    <tableColumn id="4" name="Tech_category" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Carriers_glob" displayName="Carriers_glob" ref="A32:C37" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A32:C37" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Carriers_glob" displayName="Carriers_glob" ref="A32:C37" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A32:C37"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Carrier" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Carr_name" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Carr_type" dataDxfId="5"/>
+    <tableColumn id="2" name="Carrier" dataDxfId="7"/>
+    <tableColumn id="3" name="Carr_name" dataDxfId="6"/>
+    <tableColumn id="1" name="Carr_type" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Timesteps" displayName="Timesteps" ref="A40:C44" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A40:C44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Timesteps" displayName="Timesteps" ref="A40:C44" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A40:C44"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Timeslice" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Timeslice_name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Timeslice_fraction" dataDxfId="0"/>
+    <tableColumn id="1" name="Timeslice" dataDxfId="2"/>
+    <tableColumn id="2" name="Timeslice_name" dataDxfId="1"/>
+    <tableColumn id="3" name="Timeslice_fraction" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -823,43 +987,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:C44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="34.5" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.3125" customWidth="1"/>
+    <col min="2" max="2" width="24.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.734375" customWidth="1"/>
+    <col min="6" max="6" width="34.578125" customWidth="1"/>
+    <col min="7" max="7" width="16.578125" customWidth="1"/>
+    <col min="8" max="8" width="17.3671875" customWidth="1"/>
+    <col min="9" max="9" width="16.26171875" customWidth="1"/>
+    <col min="10" max="10" width="18.20703125" customWidth="1"/>
+    <col min="11" max="11" width="19.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="8"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -868,177 +1040,335 @@
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="10" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0.35753424657534244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="11">
+        <v>0.35753424657534244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0.14246575342465753</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0.14246575342465753</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1050,4 +1380,254 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100241E96938535DD4B921FCDFB54345D30" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2dfcd6e708d07654f9ef039e0eb4800">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e" xmlns:ns3="e67e9a88-35e1-4b39-8da9-a609eb308282" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d0e77208158cc8ba8661a0337015ee0" ns2:_="" ns3:_="">
+    <xsd:import namespace="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
+    <xsd:import namespace="e67e9a88-35e1-4b39-8da9-a609eb308282"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e67e9a88-35e1-4b39-8da9-a609eb308282" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDA1C43B-E35B-48A4-8454-96BEF8B98FC4}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DA7CF7-8C87-4AED-98A0-4720646B44A7}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ACD5296-120D-41B4-8B5C-74E34A874847}"/>
 </file>
</xml_diff>